<commit_message>
built out functions to generate a random character and added documentation.
</commit_message>
<xml_diff>
--- a/src/names.xlsx
+++ b/src/names.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\projects\Programming Projects\Python Projects\Rogue Trader Game\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\projects\Programming Projects\Python Projects\Rogue Trader Game\python src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FFE28C-A1E3-490F-9EF8-796BC3795795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0993CFB-B059-42AD-A021-03A76E7EE12E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1000CD60-218C-4BFF-8646-9C2501253D3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{1000CD60-218C-4BFF-8646-9C2501253D3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Death World Names" sheetId="1" r:id="rId1"/>
-    <sheet name="Noble Born World Names" sheetId="9" r:id="rId2"/>
-    <sheet name="Imperial World Names" sheetId="8" r:id="rId3"/>
-    <sheet name="Hive World Names" sheetId="7" r:id="rId4"/>
-    <sheet name="Forge World Names" sheetId="6" r:id="rId5"/>
-    <sheet name="Void Born Names" sheetId="5" r:id="rId6"/>
+    <sheet name="Death World" sheetId="1" r:id="rId1"/>
+    <sheet name="Noble Born World" sheetId="9" r:id="rId2"/>
+    <sheet name="Imperial World" sheetId="8" r:id="rId3"/>
+    <sheet name="Hive World" sheetId="7" r:id="rId4"/>
+    <sheet name="Forge World" sheetId="6" r:id="rId5"/>
+    <sheet name="Void Born" sheetId="5" r:id="rId6"/>
     <sheet name="human male names" sheetId="2" r:id="rId7"/>
     <sheet name="human last names" sheetId="4" r:id="rId8"/>
     <sheet name="human female names" sheetId="3" r:id="rId9"/>
@@ -8838,8 +8838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A474F8-83F3-4592-986D-9712911328A2}">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F133"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10810,8 +10810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360D5431-82B9-4172-A172-0DFA619DEFE5}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>